<commit_message>
EDIT: cambios de nombre en documentos
</commit_message>
<xml_diff>
--- a/5_Profiling/TLP_final.xlsx
+++ b/5_Profiling/TLP_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barre\Documents\UPC\GIA\Q3\MEstadistica\spotify\PMAAD\5_Profiling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8FFFEC-E63D-4C96-A7A8-F151D95F659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC5E60-7A90-478E-A37B-8E9DDC3F6B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12021" yWindow="0" windowWidth="12021" windowHeight="12922" xr2:uid="{2CE78E48-E006-4825-AE88-851FB6B1AB14}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{2CE78E48-E006-4825-AE88-851FB6B1AB14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>album_type</t>
   </si>
@@ -62,15 +62,9 @@
     <t>major_mode</t>
   </si>
   <si>
-    <t>rank_group</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
-    <t>is_group</t>
-  </si>
-  <si>
     <t>artist_num</t>
   </si>
   <si>
@@ -80,25 +74,10 @@
     <t>artist_popularity</t>
   </si>
   <si>
-    <t>danceability</t>
-  </si>
-  <si>
-    <t>energy</t>
-  </si>
-  <si>
     <t>loudness</t>
   </si>
   <si>
-    <t>speechiness</t>
-  </si>
-  <si>
-    <t>acousticness</t>
-  </si>
-  <si>
     <t>valence</t>
-  </si>
-  <si>
-    <t>streams</t>
   </si>
   <si>
     <t>C1</t>
@@ -137,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +147,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -192,6 +177,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42228ED5-CE5E-439C-8750-81E715FE4C6B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -528,24 +515,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
@@ -555,7 +542,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="2"/>
@@ -565,7 +552,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="2"/>
@@ -575,183 +562,121 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-    </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>